<commit_message>
Stats classes CSVWritter, Result, StatisticsCollector were added
</commit_message>
<xml_diff>
--- a/Trie/src/main/resources/trieStats.xlsx
+++ b/Trie/src/main/resources/trieStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timur\IdeaProjects\semestrovaya02\Trie\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE8FFB4-92B9-46BC-ACD5-020E3C7CCDAD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98152A1D-ED52-4678-9A47-C77A94832D80}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10380" xr2:uid="{AC7EDAF0-E7E1-4E3B-B58A-99D313F9E12A}"/>
   </bookViews>
@@ -3415,7 +3415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1A442AC-276A-4A7E-B7D0-506291B57CD2}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>

</xml_diff>